<commit_message>
Update with descriptions of variable R and C
</commit_message>
<xml_diff>
--- a/BOM/DifferentialProbe_BOM.xlsx
+++ b/BOM/DifferentialProbe_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\differentialprobe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9561C9-3F41-4D2B-8C1D-250166E8E59D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A946F6ED-0C40-4A6A-AE31-D79BDE35B138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E3A118C5-7006-4B20-A7E3-A6155B08E887}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E3A118C5-7006-4B20-A7E3-A6155B08E887}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_THT" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="213">
   <si>
     <t>Component</t>
   </si>
@@ -642,6 +642,30 @@
   </si>
   <si>
     <t>Original Part shows T-102 YN</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack</t>
+  </si>
+  <si>
+    <t>Variable capacitor for adjusting square wave compensation and high frequency CMRR</t>
+  </si>
+  <si>
+    <t>Variable capacitor for adjusting square wave compensation.</t>
+  </si>
+  <si>
+    <t>Variable resistor for adjusting low frequency CMRR.</t>
+  </si>
+  <si>
+    <t>Variable resistor for adjusting offset when SW1 at attenuation 1/10.</t>
+  </si>
+  <si>
+    <t>Variable resistor for adjusting accuracy.</t>
+  </si>
+  <si>
+    <t>Variable resistor for adjusting offset when SW1 at attenuation 1/100.</t>
   </si>
 </sst>
 </file>
@@ -1402,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1616251-8525-4B67-B675-9B38FD7CA7B8}">
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1440,7 @@
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1632,6 +1656,9 @@
       <c r="D11" t="s">
         <v>51</v>
       </c>
+      <c r="G11" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1697,6 +1724,9 @@
       <c r="D15" t="s">
         <v>51</v>
       </c>
+      <c r="G15" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2381,7 +2411,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>131</v>
       </c>
@@ -2395,7 +2425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>177</v>
       </c>
@@ -2409,7 +2439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>178</v>
       </c>
@@ -2423,7 +2453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>179</v>
       </c>
@@ -2437,7 +2467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>180</v>
       </c>
@@ -2451,7 +2481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>181</v>
       </c>
@@ -2465,7 +2495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>182</v>
       </c>
@@ -2476,7 +2506,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>189</v>
       </c>
@@ -2490,7 +2520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -2504,7 +2534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>194</v>
       </c>
@@ -2518,7 +2548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>195</v>
       </c>
@@ -2532,7 +2562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>196</v>
       </c>
@@ -2546,7 +2576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>197</v>
       </c>
@@ -2560,7 +2590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>198</v>
       </c>
@@ -2574,7 +2604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
@@ -2587,8 +2617,11 @@
       <c r="F79" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>117</v>
       </c>
@@ -2600,6 +2633,9 @@
       </c>
       <c r="F80" t="s">
         <v>11</v>
+      </c>
+      <c r="G80" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2615,6 +2651,9 @@
       <c r="F81" t="s">
         <v>11</v>
       </c>
+      <c r="G81" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -2629,6 +2668,9 @@
       <c r="F82" t="s">
         <v>11</v>
       </c>
+      <c r="G82" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -3043,6 +3085,17 @@
       </c>
       <c r="H111" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>205</v>
+      </c>
+      <c r="C112" t="s">
+        <v>206</v>
+      </c>
+      <c r="F112" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3394,7 +3447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00FE661-8528-479E-9AE8-CCEA0E0C44CF}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
draft design and BOM started
</commit_message>
<xml_diff>
--- a/BOM/DifferentialProbe_BOM.xlsx
+++ b/BOM/DifferentialProbe_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\differentialprobe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A946F6ED-0C40-4A6A-AE31-D79BDE35B138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF46FED-BBAB-45AF-958F-5AD2EC13DA7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E3A118C5-7006-4B20-A7E3-A6155B08E887}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="BOM_SMT" sheetId="3" r:id="rId2"/>
     <sheet name="Lists" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM_THT!$A$1:$M$112</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="235">
   <si>
     <t>Component</t>
   </si>
@@ -230,9 +233,6 @@
     <t>C40</t>
   </si>
   <si>
-    <t>n/f</t>
-  </si>
-  <si>
     <t>C41</t>
   </si>
   <si>
@@ -323,9 +323,6 @@
     <t>U441NL</t>
   </si>
   <si>
-    <t>2N3958</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -666,13 +663,88 @@
   </si>
   <si>
     <t>Variable resistor for adjusting offset when SW1 at attenuation 1/100.</t>
+  </si>
+  <si>
+    <t>Slide Switch, SPDT, Through Hole, SSSF Series, 100 mA (farnell.com)</t>
+  </si>
+  <si>
+    <t>SW1,2</t>
+  </si>
+  <si>
+    <t>DC Power Connector, Receptacle, 2.1 mm, PCB Mount, Solder (farnell.com)</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>HFA3046BZ</t>
+  </si>
+  <si>
+    <t>Bipolar Transistor Array, NPN, 12 V, 34 mA, 150 mW, 40 hFE, SOIC (farnell.com)</t>
+  </si>
+  <si>
+    <t>Typo in schematic, part is LM3046M instead of LM3406M</t>
+  </si>
+  <si>
+    <t>Other have seen 2N3958</t>
+  </si>
+  <si>
+    <t>IFN411 InterFET | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>IFN441</t>
+  </si>
+  <si>
+    <t>Not Fitted</t>
+  </si>
+  <si>
+    <t>Through Hole Resistor, 1 Mohm, R Series, 250 mW, ± 0.1%, Axial Leaded, 500 V (farnell.com)</t>
+  </si>
+  <si>
+    <t>R1a,1b,2a,2b,3a,3b,4a,4c</t>
+  </si>
+  <si>
+    <t>R5,6</t>
+  </si>
+  <si>
+    <t>Through Hole Resistor, 26.1 kohm, MCMF0W4 Series, 250 mW, ± 0.5%, Axial Leaded, 250 V (farnell.com)</t>
+  </si>
+  <si>
+    <t>Trimpot, Multi Turn, Cermet, Top Adjust, 500 ohm, Through Hole, 23 Turns (farnell.com)</t>
+  </si>
+  <si>
+    <t>HSE682SAQCF0KR Vishay / Draloric | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>CC45SL3AD121JYVNA TDK | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>CC45SL3AD820JYNNA TDK | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>JZ300 Knowles Voltronics | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>Small Signal Diode, Single, 100 V, 200 mA, 1 V, 4 ns, 1 A (farnell.com)</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor, 0.1 uF, 50 V, Mono-Kap Series, ± 10%, Radial Leaded, X7R (farnell.com)</t>
+  </si>
+  <si>
+    <t>Through Hole Resistor, 680 ohm, MF25 Series, 250 mW, ± 1%, Axial Leaded, 250 V (farnell.com)</t>
+  </si>
+  <si>
+    <t>C16,19,20,21,26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,6 +762,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -712,15 +792,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
@@ -1426,27 +1523,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1616251-8525-4B67-B675-9B38FD7CA7B8}">
-  <dimension ref="A1:N112"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,37 +1558,34 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="7" t="s">
+        <v>133</v>
+      </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1503,11 +1598,17 @@
       <c r="D2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I2">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1520,11 +1621,17 @@
       <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I3">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1537,11 +1644,17 @@
       <c r="D4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1554,11 +1667,17 @@
       <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1571,11 +1690,17 @@
       <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1588,11 +1713,17 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="I7">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1605,11 +1736,17 @@
       <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I8">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1622,11 +1759,17 @@
       <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I9">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1639,11 +1782,17 @@
       <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1656,11 +1805,17 @@
       <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="G11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I11">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1673,11 +1828,17 @@
       <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I12">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1690,11 +1851,17 @@
       <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I13">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1707,11 +1874,17 @@
       <c r="D14" t="s">
         <v>49</v>
       </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I14">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1724,25 +1897,40 @@
       <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c r="G15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I15">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
+      <c r="B16" t="s">
+        <v>234</v>
+      </c>
       <c r="C16" t="s">
         <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I16">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1752,11 +1940,11 @@
       <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1766,53 +1954,80 @@
       <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
+      <c r="B19" t="s">
+        <v>234</v>
+      </c>
       <c r="C19" t="s">
         <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I19">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
+      <c r="B20" t="s">
+        <v>234</v>
+      </c>
       <c r="C20" t="s">
         <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I20">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
+      <c r="B21" t="s">
+        <v>234</v>
+      </c>
       <c r="C21" t="s">
         <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I21">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1822,11 +2037,11 @@
       <c r="D22" t="s">
         <v>59</v>
       </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1836,11 +2051,11 @@
       <c r="D23" t="s">
         <v>58</v>
       </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1850,69 +2065,78 @@
       <c r="D24" t="s">
         <v>58</v>
       </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
+      <c r="B25" t="s">
+        <v>234</v>
+      </c>
       <c r="C25" t="s">
         <v>63</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
       </c>
-      <c r="F25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I25">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1922,11 +2146,11 @@
       <c r="D29" t="s">
         <v>57</v>
       </c>
-      <c r="F29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1936,25 +2160,25 @@
       <c r="D30" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1964,11 +2188,11 @@
       <c r="D32" t="s">
         <v>57</v>
       </c>
-      <c r="F32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1976,1132 +2200,1354 @@
         <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>221</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
       <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
         <v>69</v>
       </c>
-      <c r="D36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
-      <c r="C38" t="s">
+      <c r="B39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
         <v>83</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I39">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I40">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>223</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I41">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>223</v>
+      </c>
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I42">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I43">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I44">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>223</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="I45">
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C46" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I46">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I47">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" t="s">
+        <v>140</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" t="s">
+        <v>141</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I55">
+        <v>3.85E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I57">
+        <v>3.85E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" t="s">
+        <v>142</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" t="s">
+        <v>130</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" t="s">
+        <v>130</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" t="s">
+        <v>185</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" t="s">
+        <v>183</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" t="s">
+        <v>182</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>187</v>
+      </c>
+      <c r="C72" t="s">
+        <v>82</v>
+      </c>
+      <c r="D72" t="s">
+        <v>188</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>191</v>
+      </c>
+      <c r="C73" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>192</v>
+      </c>
+      <c r="C74" t="s">
+        <v>82</v>
+      </c>
+      <c r="D74" t="s">
+        <v>137</v>
+      </c>
+      <c r="E74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>193</v>
+      </c>
+      <c r="C75" t="s">
+        <v>82</v>
+      </c>
+      <c r="D75" t="s">
+        <v>188</v>
+      </c>
+      <c r="E75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" t="s">
+        <v>140</v>
+      </c>
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>195</v>
+      </c>
+      <c r="C77" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77" t="s">
+        <v>182</v>
+      </c>
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>196</v>
+      </c>
+      <c r="C78" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
+        <v>92</v>
+      </c>
+      <c r="D79" t="s">
+        <v>93</v>
+      </c>
+      <c r="E79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="I79">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>135</v>
+      </c>
+      <c r="C81" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" t="s">
+        <v>93</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" t="s">
+        <v>95</v>
+      </c>
+      <c r="D83" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I83">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" t="s">
+        <v>118</v>
+      </c>
+      <c r="D84" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G84" t="s">
+        <v>215</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="I84">
+        <v>10.49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" t="s">
+        <v>132</v>
+      </c>
+      <c r="E85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" t="s">
+        <v>165</v>
+      </c>
+      <c r="D86" t="s">
+        <v>166</v>
+      </c>
+      <c r="E86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>84</v>
       </c>
-      <c r="F38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" t="s">
-        <v>84</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" t="s">
-        <v>83</v>
-      </c>
-      <c r="D43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" t="s">
-        <v>91</v>
-      </c>
-      <c r="F46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" t="s">
-        <v>91</v>
-      </c>
-      <c r="F47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" t="s">
-        <v>83</v>
-      </c>
-      <c r="D48" t="s">
-        <v>140</v>
-      </c>
-      <c r="F48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" t="s">
-        <v>119</v>
-      </c>
-      <c r="F49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D50" t="s">
-        <v>125</v>
-      </c>
-      <c r="F50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" t="s">
-        <v>83</v>
-      </c>
-      <c r="D52" t="s">
-        <v>142</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C87" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>87</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I87">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="C88" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88" t="s">
+        <v>87</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="I88">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>121</v>
+      </c>
+      <c r="C89" t="s">
+        <v>86</v>
+      </c>
+      <c r="D89" t="s">
+        <v>122</v>
+      </c>
+      <c r="E89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>143</v>
       </c>
-      <c r="F53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" t="s">
-        <v>143</v>
-      </c>
-      <c r="F54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" t="s">
-        <v>83</v>
-      </c>
-      <c r="D55" t="s">
-        <v>110</v>
-      </c>
-      <c r="F55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" t="s">
-        <v>83</v>
-      </c>
-      <c r="D56" t="s">
-        <v>126</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>83</v>
-      </c>
-      <c r="D57" t="s">
-        <v>110</v>
-      </c>
-      <c r="F57" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" t="s">
-        <v>83</v>
-      </c>
-      <c r="D58" t="s">
-        <v>126</v>
-      </c>
-      <c r="F58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" t="s">
-        <v>83</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C90" t="s">
+        <v>86</v>
+      </c>
+      <c r="D90" t="s">
+        <v>87</v>
+      </c>
+      <c r="E90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>144</v>
       </c>
-      <c r="F59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>115</v>
-      </c>
-      <c r="C60" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" t="s">
-        <v>122</v>
-      </c>
-      <c r="F60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" t="s">
-        <v>83</v>
-      </c>
-      <c r="D61" t="s">
-        <v>127</v>
-      </c>
-      <c r="F61" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>83</v>
-      </c>
-      <c r="D62" t="s">
-        <v>132</v>
-      </c>
-      <c r="F62" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" t="s">
-        <v>83</v>
-      </c>
-      <c r="D63" t="s">
-        <v>132</v>
-      </c>
-      <c r="F63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" t="s">
-        <v>187</v>
-      </c>
-      <c r="F64" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" t="s">
-        <v>83</v>
-      </c>
-      <c r="D65" t="s">
-        <v>139</v>
-      </c>
-      <c r="F65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>177</v>
-      </c>
-      <c r="C66" t="s">
-        <v>83</v>
-      </c>
-      <c r="D66" t="s">
-        <v>188</v>
-      </c>
-      <c r="F66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>178</v>
-      </c>
-      <c r="C67" t="s">
-        <v>83</v>
-      </c>
-      <c r="D67" t="s">
-        <v>185</v>
-      </c>
-      <c r="F67" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>179</v>
-      </c>
-      <c r="C68" t="s">
-        <v>83</v>
-      </c>
-      <c r="D68" t="s">
-        <v>186</v>
-      </c>
-      <c r="F68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>180</v>
-      </c>
-      <c r="C69" t="s">
-        <v>83</v>
-      </c>
-      <c r="D69" t="s">
-        <v>183</v>
-      </c>
-      <c r="F69" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>181</v>
-      </c>
-      <c r="C70" t="s">
-        <v>83</v>
-      </c>
-      <c r="D70" t="s">
-        <v>184</v>
-      </c>
-      <c r="F70" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C91" t="s">
+        <v>86</v>
+      </c>
+      <c r="D91" t="s">
+        <v>87</v>
+      </c>
+      <c r="E91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>145</v>
+      </c>
+      <c r="C92" t="s">
+        <v>86</v>
+      </c>
+      <c r="D92" t="s">
+        <v>168</v>
+      </c>
+      <c r="E92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>146</v>
+      </c>
+      <c r="C93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93" t="s">
+        <v>168</v>
+      </c>
+      <c r="E93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94" t="s">
+        <v>86</v>
+      </c>
+      <c r="D94" t="s">
+        <v>87</v>
+      </c>
+      <c r="E94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" t="s">
+        <v>86</v>
+      </c>
+      <c r="D95" t="s">
+        <v>87</v>
+      </c>
+      <c r="E95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>149</v>
+      </c>
+      <c r="C96" t="s">
+        <v>86</v>
+      </c>
+      <c r="D96" t="s">
+        <v>87</v>
+      </c>
+      <c r="E96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>150</v>
+      </c>
+      <c r="C97" t="s">
+        <v>86</v>
+      </c>
+      <c r="D97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>167</v>
+      </c>
+      <c r="C98" t="s">
+        <v>173</v>
+      </c>
+      <c r="D98" t="s">
+        <v>174</v>
+      </c>
+      <c r="E98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>169</v>
+      </c>
+      <c r="C99" t="s">
+        <v>173</v>
+      </c>
+      <c r="D99" t="s">
+        <v>174</v>
+      </c>
+      <c r="E99" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>170</v>
+      </c>
+      <c r="C100" t="s">
+        <v>173</v>
+      </c>
+      <c r="D100" t="s">
+        <v>174</v>
+      </c>
+      <c r="E100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>171</v>
+      </c>
+      <c r="C101" t="s">
+        <v>173</v>
+      </c>
+      <c r="D101" t="s">
+        <v>174</v>
+      </c>
+      <c r="E101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>172</v>
+      </c>
+      <c r="C102" t="s">
+        <v>173</v>
+      </c>
+      <c r="D102" t="s">
+        <v>174</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" t="s">
+        <v>200</v>
+      </c>
+      <c r="D103" t="s">
+        <v>201</v>
+      </c>
+      <c r="E103" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>151</v>
+      </c>
+      <c r="C104" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" t="s">
+        <v>158</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>152</v>
+      </c>
+      <c r="C105" t="s">
+        <v>157</v>
+      </c>
+      <c r="D105" t="s">
+        <v>159</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>153</v>
+      </c>
+      <c r="C106" t="s">
+        <v>190</v>
+      </c>
+      <c r="D106" t="s">
         <v>189</v>
       </c>
-      <c r="C72" t="s">
-        <v>83</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>154</v>
+      </c>
+      <c r="C107" t="s">
+        <v>157</v>
+      </c>
+      <c r="D107" t="s">
+        <v>198</v>
+      </c>
+      <c r="E107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>155</v>
+      </c>
+      <c r="C108" t="s">
         <v>190</v>
       </c>
-      <c r="F72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" t="s">
-        <v>199</v>
-      </c>
-      <c r="F73" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>194</v>
-      </c>
-      <c r="C74" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" t="s">
-        <v>139</v>
-      </c>
-      <c r="F74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" t="s">
-        <v>83</v>
-      </c>
-      <c r="D75" t="s">
-        <v>190</v>
-      </c>
-      <c r="F75" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>196</v>
-      </c>
-      <c r="C76" t="s">
-        <v>83</v>
-      </c>
-      <c r="D76" t="s">
-        <v>142</v>
-      </c>
-      <c r="F76" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>197</v>
-      </c>
-      <c r="C77" t="s">
-        <v>83</v>
-      </c>
-      <c r="D77" t="s">
-        <v>184</v>
-      </c>
-      <c r="F77" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>198</v>
-      </c>
-      <c r="C78" t="s">
-        <v>83</v>
-      </c>
-      <c r="D78" t="s">
-        <v>142</v>
-      </c>
-      <c r="F78" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>92</v>
-      </c>
-      <c r="C79" t="s">
-        <v>93</v>
-      </c>
-      <c r="D79" t="s">
-        <v>94</v>
-      </c>
-      <c r="F79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>117</v>
-      </c>
-      <c r="C80" t="s">
-        <v>93</v>
-      </c>
-      <c r="D80" t="s">
-        <v>118</v>
-      </c>
-      <c r="F80" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" t="s">
+      <c r="D108" t="s">
+        <v>189</v>
+      </c>
+      <c r="E108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>156</v>
+      </c>
+      <c r="C109" t="s">
+        <v>157</v>
+      </c>
+      <c r="D109" t="s">
+        <v>158</v>
+      </c>
+      <c r="E109" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>160</v>
+      </c>
+      <c r="B110" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" t="s">
-        <v>93</v>
-      </c>
-      <c r="D81" t="s">
-        <v>94</v>
-      </c>
-      <c r="F81" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" t="s">
+      <c r="C110" t="s">
+        <v>163</v>
+      </c>
+      <c r="E110" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="H110" s="3" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>138</v>
-      </c>
-      <c r="C82" t="s">
-        <v>93</v>
-      </c>
-      <c r="D82" t="s">
-        <v>139</v>
-      </c>
-      <c r="F82" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>95</v>
-      </c>
-      <c r="C83" t="s">
-        <v>96</v>
-      </c>
-      <c r="D83" t="s">
-        <v>97</v>
-      </c>
-      <c r="F83" t="s">
-        <v>12</v>
-      </c>
-      <c r="H83" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>99</v>
-      </c>
-      <c r="C84" t="s">
-        <v>120</v>
-      </c>
-      <c r="D84" t="s">
-        <v>121</v>
-      </c>
-      <c r="F84" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>100</v>
-      </c>
-      <c r="C85" t="s">
-        <v>133</v>
-      </c>
-      <c r="D85" t="s">
-        <v>134</v>
-      </c>
-      <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="H85" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>101</v>
-      </c>
-      <c r="C86" t="s">
-        <v>167</v>
-      </c>
-      <c r="D86" t="s">
-        <v>168</v>
-      </c>
-      <c r="F86" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>85</v>
-      </c>
-      <c r="C87" t="s">
-        <v>87</v>
-      </c>
-      <c r="D87" t="s">
-        <v>88</v>
-      </c>
-      <c r="F87" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>86</v>
-      </c>
-      <c r="C88" t="s">
-        <v>87</v>
-      </c>
-      <c r="D88" t="s">
-        <v>88</v>
-      </c>
-      <c r="F88" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" t="s">
-        <v>87</v>
-      </c>
-      <c r="D89" t="s">
-        <v>124</v>
-      </c>
-      <c r="F89" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>145</v>
-      </c>
-      <c r="C90" t="s">
-        <v>87</v>
-      </c>
-      <c r="D90" t="s">
-        <v>88</v>
-      </c>
-      <c r="F90" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>146</v>
-      </c>
-      <c r="C91" t="s">
-        <v>87</v>
-      </c>
-      <c r="D91" t="s">
-        <v>88</v>
-      </c>
-      <c r="F91" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>147</v>
-      </c>
-      <c r="C92" t="s">
-        <v>87</v>
-      </c>
-      <c r="D92" t="s">
-        <v>170</v>
-      </c>
-      <c r="F92" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>148</v>
-      </c>
-      <c r="C93" t="s">
-        <v>87</v>
-      </c>
-      <c r="D93" t="s">
-        <v>170</v>
-      </c>
-      <c r="F93" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>149</v>
-      </c>
-      <c r="C94" t="s">
-        <v>87</v>
-      </c>
-      <c r="D94" t="s">
-        <v>88</v>
-      </c>
-      <c r="F94" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>150</v>
-      </c>
-      <c r="C95" t="s">
-        <v>87</v>
-      </c>
-      <c r="D95" t="s">
-        <v>88</v>
-      </c>
-      <c r="F95" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>151</v>
-      </c>
-      <c r="C96" t="s">
-        <v>87</v>
-      </c>
-      <c r="D96" t="s">
-        <v>88</v>
-      </c>
-      <c r="F96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>152</v>
-      </c>
-      <c r="C97" t="s">
-        <v>87</v>
-      </c>
-      <c r="D97" t="s">
-        <v>88</v>
-      </c>
-      <c r="F97" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>169</v>
-      </c>
-      <c r="C98" t="s">
-        <v>175</v>
-      </c>
-      <c r="D98" t="s">
-        <v>176</v>
-      </c>
-      <c r="F98" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>171</v>
-      </c>
-      <c r="C99" t="s">
-        <v>175</v>
-      </c>
-      <c r="D99" t="s">
-        <v>176</v>
-      </c>
-      <c r="F99" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>172</v>
-      </c>
-      <c r="C100" t="s">
-        <v>175</v>
-      </c>
-      <c r="D100" t="s">
-        <v>176</v>
-      </c>
-      <c r="F100" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>173</v>
-      </c>
-      <c r="C101" t="s">
-        <v>175</v>
-      </c>
-      <c r="D101" t="s">
-        <v>176</v>
-      </c>
-      <c r="F101" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>174</v>
-      </c>
-      <c r="C102" t="s">
-        <v>175</v>
-      </c>
-      <c r="D102" t="s">
-        <v>176</v>
-      </c>
-      <c r="F102" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>201</v>
-      </c>
-      <c r="C103" t="s">
-        <v>202</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="I110">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" t="s">
+        <v>212</v>
+      </c>
+      <c r="C111" t="s">
+        <v>163</v>
+      </c>
+      <c r="E111" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="I111">
+        <v>0.72399999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>203</v>
       </c>
-      <c r="F103" t="s">
-        <v>12</v>
-      </c>
-      <c r="H103" t="s">
+      <c r="C112" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>153</v>
-      </c>
-      <c r="C104" t="s">
-        <v>159</v>
-      </c>
-      <c r="D104" t="s">
-        <v>160</v>
-      </c>
-      <c r="F104" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>154</v>
-      </c>
-      <c r="C105" t="s">
-        <v>159</v>
-      </c>
-      <c r="D105" t="s">
-        <v>161</v>
-      </c>
-      <c r="F105" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>155</v>
-      </c>
-      <c r="C106" t="s">
-        <v>192</v>
-      </c>
-      <c r="D106" t="s">
-        <v>191</v>
-      </c>
-      <c r="F106" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>156</v>
-      </c>
-      <c r="C107" t="s">
-        <v>159</v>
-      </c>
-      <c r="D107" t="s">
-        <v>200</v>
-      </c>
-      <c r="F107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>157</v>
-      </c>
-      <c r="C108" t="s">
-        <v>192</v>
-      </c>
-      <c r="D108" t="s">
-        <v>191</v>
-      </c>
-      <c r="F108" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>158</v>
-      </c>
-      <c r="C109" t="s">
-        <v>159</v>
-      </c>
-      <c r="D109" t="s">
-        <v>160</v>
-      </c>
-      <c r="F109" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>162</v>
-      </c>
-      <c r="C110" t="s">
-        <v>165</v>
-      </c>
-      <c r="F110" t="s">
-        <v>12</v>
-      </c>
-      <c r="H110" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>163</v>
-      </c>
-      <c r="C111" t="s">
-        <v>165</v>
-      </c>
-      <c r="F111" t="s">
-        <v>12</v>
-      </c>
-      <c r="H111" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>205</v>
-      </c>
-      <c r="C112" t="s">
-        <v>206</v>
-      </c>
-      <c r="F112" t="s">
-        <v>11</v>
+      <c r="E112" t="s">
+        <v>11</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I112">
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H116" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I116" s="5">
+        <f>SUM(I2:I112)</f>
+        <v>54.746000000000002</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M112" xr:uid="{AE3DD381-F2B7-403A-B289-727EF6C0D84E}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H110" r:id="rId1" display="https://be.farnell.com/alps-alpine/sssf011700/slide-switch-spdt-0-1a-30v-tht/dp/3261774?st=switch%20slide" xr:uid="{D0D6BEF2-996F-4A06-B35A-02EEEC80A8AA}"/>
+    <hyperlink ref="H111" r:id="rId2" display="https://be.farnell.com/alps-alpine/sssf011700/slide-switch-spdt-0-1a-30v-tht/dp/3261774?st=switch%20slide" xr:uid="{F442F32C-8502-42BE-AB56-A742441952D8}"/>
+    <hyperlink ref="H112" r:id="rId3" display="https://be.farnell.com/pro-power/ppw01010/2-1mm-dc-socket-locking/dp/3498419?st=dc%20barrel%20jack" xr:uid="{8C7C4A37-7AA0-4906-AF82-90CF878D4023}"/>
+    <hyperlink ref="H84" r:id="rId4" display="https://be.farnell.com/renesas/hfa3046bz/transistor-npn-12v-0-15w-soic/dp/2983709?ost=hfa3046" xr:uid="{9EC2271E-74B8-4F63-945C-48C162315737}"/>
+    <hyperlink ref="H83" r:id="rId5" display="https://www.mouser.be/ProductDetail/InterFET/IFN411?qs=ggD623E1wpTqTvB4DJqgbw%3D%3D" xr:uid="{5465D79E-22EB-4CAB-AE87-A15EBCEDBA33}"/>
+    <hyperlink ref="H38" r:id="rId6" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{3F3C68F7-2183-4729-9923-81D054D613B9}"/>
+    <hyperlink ref="H39" r:id="rId7" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{52F3F128-6F80-4E7E-8496-5C05CA8B6E8E}"/>
+    <hyperlink ref="H40" r:id="rId8" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{2976635D-4B56-488B-949D-241B58187194}"/>
+    <hyperlink ref="H41" r:id="rId9" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{DA35A531-5414-4B9C-A549-0720A7830C59}"/>
+    <hyperlink ref="H42" r:id="rId10" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{3BB61933-654B-4C0D-9FB5-1240AB91FDBF}"/>
+    <hyperlink ref="H43" r:id="rId11" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{7F69FAAD-FFBF-4F81-82DD-3FD03116926E}"/>
+    <hyperlink ref="H44" r:id="rId12" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{97983E24-B3F5-4F72-BEDD-0199498168E4}"/>
+    <hyperlink ref="H45" r:id="rId13" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{6B2B45C4-DDA1-4F69-ADB1-D8463EED1C77}"/>
+    <hyperlink ref="H46" r:id="rId14" display="https://be.farnell.com/multicomp/mcmf0w4df2612a50/res-26k1-0-50-250mw-axial/dp/1563153" xr:uid="{641175BA-9D50-494D-A430-C85D7B350545}"/>
+    <hyperlink ref="H47" r:id="rId15" display="https://be.farnell.com/multicomp/mcmf0w4df2612a50/res-26k1-0-50-250mw-axial/dp/1563153" xr:uid="{8B4EF911-20E9-4125-A430-3AE0C07DF73A}"/>
+    <hyperlink ref="H79" r:id="rId16" display="https://be.farnell.com/vishay/t93yb501kt20/trimmer-pot-500r-23turn-thd/dp/1141414?st=trimpot" xr:uid="{CD773C5A-2FF2-47B0-96ED-D7D84F9F24A8}"/>
+    <hyperlink ref="H2" r:id="rId17" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{5760DDC1-F974-4B8F-8172-E6C89F2DC67A}"/>
+    <hyperlink ref="H3" r:id="rId18" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{9B6162F1-074B-454D-AFDB-754BA66A8BA1}"/>
+    <hyperlink ref="H4" r:id="rId19" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{3EDED0DE-88D0-4B5E-8D01-6249EF594A0B}"/>
+    <hyperlink ref="H5" r:id="rId20" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{915C0B1E-E8A4-4807-8F02-3F6DCDB4144D}"/>
+    <hyperlink ref="H6" r:id="rId21" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{E45E5087-FCBA-497D-99BD-5805EDB8BD6B}"/>
+    <hyperlink ref="H7" r:id="rId22" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{2F272D9E-C2FB-460D-9B6D-66C248CC18A0}"/>
+    <hyperlink ref="H8" r:id="rId23" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD121JYVNA?qs=eSfX1CQlHqq1jQpjjENGKQ%3D%3D" xr:uid="{F17337F9-8F48-4F04-98B9-796C15E925E9}"/>
+    <hyperlink ref="H12" r:id="rId24" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD121JYVNA?qs=eSfX1CQlHqq1jQpjjENGKQ%3D%3D" xr:uid="{5E810595-7554-4FA3-883E-460F81E24968}"/>
+    <hyperlink ref="H9" r:id="rId25" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD820JYNNA?qs=2FIyTMJ0hNlY1vHleNE%252B0A%3D%3D" xr:uid="{908FA395-24A9-444B-A60A-C0772E052359}"/>
+    <hyperlink ref="H10" r:id="rId26" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD820JYNNA?qs=2FIyTMJ0hNlY1vHleNE%252B0A%3D%3D" xr:uid="{A72AC7F0-3A83-4F0D-BCDE-C609C38F2C26}"/>
+    <hyperlink ref="H13" r:id="rId27" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD820JYNNA?qs=2FIyTMJ0hNlY1vHleNE%252B0A%3D%3D" xr:uid="{5B678C36-E6E2-4003-B7C1-1FFAD8389C1F}"/>
+    <hyperlink ref="H14" r:id="rId28" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD820JYNNA?qs=2FIyTMJ0hNlY1vHleNE%252B0A%3D%3D" xr:uid="{A4E09FC9-1439-4787-A730-59EC72CE93A3}"/>
+    <hyperlink ref="H11" r:id="rId29" display="https://www.mouser.be/ProductDetail/Knowles-Voltronics/JZ300?qs=l0I8jaqwYiDrMk2Sd%252BO3uQ%3D%3D" xr:uid="{6FDE52E5-E44A-47A3-BFA8-C79F8D07A0BE}"/>
+    <hyperlink ref="H15" r:id="rId30" display="https://www.mouser.be/ProductDetail/Knowles-Voltronics/JZ300?qs=l0I8jaqwYiDrMk2Sd%252BO3uQ%3D%3D" xr:uid="{D05A97ED-9FA3-467A-B0E8-09B89E201259}"/>
+    <hyperlink ref="H87" r:id="rId31" display="https://be.farnell.com/on-semiconductor/1n4148tr/diode-100v-200ma-do-35/dp/9843680?st=1n4148" xr:uid="{29DDBB07-86F0-491F-B1DE-1595D1348EAA}"/>
+    <hyperlink ref="H88" r:id="rId32" display="https://be.farnell.com/on-semiconductor/1n4148tr/diode-100v-200ma-do-35/dp/9843680?st=1n4148" xr:uid="{DFE394BF-4AEC-4D75-97EF-94A70C1C8BE9}"/>
+    <hyperlink ref="H16" r:id="rId33" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{B01CC1CC-D2FB-4484-99F2-69412A92765F}"/>
+    <hyperlink ref="H19" r:id="rId34" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{41B0C811-66C8-4CD2-A5A2-A2DCD50CC5B0}"/>
+    <hyperlink ref="H55" r:id="rId35" display="https://be.farnell.com/multicomp/mf25-680r/res-680r-1-250mw-axial-metal-film/dp/9342150?st=680r" xr:uid="{28487200-27F9-4A59-BAC5-90632C3EEFFC}"/>
+    <hyperlink ref="H57" r:id="rId36" display="https://be.farnell.com/multicomp/mf25-680r/res-680r-1-250mw-axial-metal-film/dp/9342150?st=680r" xr:uid="{91670B6C-416D-4DDA-9A00-1DA28BC684F6}"/>
+    <hyperlink ref="H20" r:id="rId37" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{244ADBF4-02F8-402E-8BB8-45639439037B}"/>
+    <hyperlink ref="H21" r:id="rId38" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{E8A53E81-D234-491B-BB47-DD505F92D30A}"/>
+    <hyperlink ref="H25" r:id="rId39" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{77B2FCC8-BE9C-4A9B-A869-D5D7FC6E803C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -3126,7 +3572,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F23:F24 F26 F33 F28:F31 H83 H85 F92 F110:F1048576 F98:F107 F59:F89 F35:F57 F1:F18</xm:sqref>
+          <xm:sqref>E23:E24 E26 E33 E28:E31 G85 E92 E110:E1048576 E98:E107 E59:E89 E35:E57 E1:E18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="27" operator="equal" id="{4055A6CB-6532-4BB7-BD34-5F32D65F956F}">
@@ -3149,7 +3595,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F19:F21</xm:sqref>
+          <xm:sqref>E19:E21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="25" operator="equal" id="{518A8393-EE53-4B91-A5C4-A4C096C7180A}">
@@ -3172,7 +3618,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F25</xm:sqref>
+          <xm:sqref>E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="23" operator="equal" id="{A29B0310-DC02-4016-A7A0-84E1E5EE7204}">
@@ -3195,7 +3641,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F32</xm:sqref>
+          <xm:sqref>E32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="21" operator="equal" id="{568B99C1-89EF-4683-A8EC-4576D0E86404}">
@@ -3218,7 +3664,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F22</xm:sqref>
+          <xm:sqref>E22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="19" operator="equal" id="{4C90F239-37E0-41EA-858E-2FA7D7B7ACD4}">
@@ -3241,7 +3687,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F34</xm:sqref>
+          <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="17" operator="equal" id="{CA19F6AF-5125-40E8-B71B-4E25926EC801}">
@@ -3264,7 +3710,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F27</xm:sqref>
+          <xm:sqref>E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="15" operator="equal" id="{7A1174D7-CA68-44DE-B378-6FB0396088E3}">
@@ -3287,7 +3733,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F58</xm:sqref>
+          <xm:sqref>E58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="11" operator="equal" id="{030F0951-2BC6-4B2E-98E1-24E129459F63}">
@@ -3310,7 +3756,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F93</xm:sqref>
+          <xm:sqref>E93</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="9" operator="equal" id="{7C9B5E53-2A75-4702-8FFE-0FA902B0814E}">
@@ -3333,7 +3779,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F91</xm:sqref>
+          <xm:sqref>E91</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="7" operator="equal" id="{F418BD5E-A6A6-4803-98B2-2F802FADC102}">
@@ -3356,7 +3802,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F109</xm:sqref>
+          <xm:sqref>E109</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="5" operator="equal" id="{D784BC5A-8A9F-405B-9A5C-7771DCDE809C}">
@@ -3379,7 +3825,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F90</xm:sqref>
+          <xm:sqref>E90</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="3" operator="equal" id="{C5FF6173-3500-48C3-B1D3-802C6466ACCB}">
@@ -3402,7 +3848,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F108</xm:sqref>
+          <xm:sqref>E108</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="1" operator="equal" id="{D3ECBBB0-EED7-4CF4-9FBC-2F7B8B6891F9}">
@@ -3425,7 +3871,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F94:F97</xm:sqref>
+          <xm:sqref>E94:E97</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3435,7 +3881,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3485,7 +3931,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
finalized rev0 for ordering
</commit_message>
<xml_diff>
--- a/BOM/DifferentialProbe_BOM.xlsx
+++ b/BOM/DifferentialProbe_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\Documents\GitHub\differentialprobe\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5671A33-0876-4D06-9518-15FC0F963FE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FE80B5-048F-4B73-978B-F7EBF4082C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E3A118C5-7006-4B20-A7E3-A6155B08E887}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="270">
   <si>
     <t>Component</t>
   </si>
@@ -788,9 +788,6 @@
     <t>R12,13</t>
   </si>
   <si>
-    <t>Through Hole Resistor, 2.21 ohm, LR Series, 600 mW, ± 1%, Axial Leaded, 350 V (farnell.com)</t>
-  </si>
-  <si>
     <t>R15,17</t>
   </si>
   <si>
@@ -840,6 +837,9 @@
   </si>
   <si>
     <t>1C10C0G220J050B Vishay | Mouser Belgium</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-210R Yageo | Mouser Belgium</t>
   </si>
 </sst>
 </file>
@@ -1628,11 +1628,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1616251-8525-4B67-B675-9B38FD7CA7B8}">
+  <sheetPr filterMode="1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1705,7 @@
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -1728,7 +1731,7 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1754,7 +1757,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1780,7 +1783,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1806,7 +1809,7 @@
         <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -1832,7 +1835,7 @@
         <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -1858,7 +1861,7 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -1884,7 +1887,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -1910,7 +1913,7 @@
         <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -1936,7 +1939,7 @@
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" t="s">
         <v>50</v>
@@ -1962,7 +1965,7 @@
         <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -1988,7 +1991,7 @@
         <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2014,7 +2017,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2040,7 +2043,7 @@
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D15" t="s">
         <v>50</v>
@@ -2060,22 +2063,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
       </c>
       <c r="E16" t="s">
+        <v>267</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="J16">
         <v>0.15</v>
@@ -2089,7 +2092,7 @@
         <v>234</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2112,7 +2115,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2135,7 +2138,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2161,7 +2164,7 @@
         <v>234</v>
       </c>
       <c r="C20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2187,7 +2190,7 @@
         <v>234</v>
       </c>
       <c r="C21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -2213,7 +2216,7 @@
         <v>234</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2236,7 +2239,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -2248,7 +2251,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J23">
         <v>0.28999999999999998</v>
@@ -2259,10 +2262,10 @@
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2272,6 +2275,12 @@
       </c>
       <c r="F24" t="s">
         <v>11</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J24">
+        <v>0.46</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2279,10 +2288,10 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -2294,7 +2303,7 @@
         <v>11</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J25">
         <v>0.46</v>
@@ -2308,7 +2317,7 @@
         <v>234</v>
       </c>
       <c r="C26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -2326,7 +2335,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2343,7 +2352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2361,7 +2370,7 @@
       </c>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2379,7 +2388,7 @@
       </c>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2396,7 +2405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2430,7 +2439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2447,7 +2456,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2464,7 +2473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -2487,7 +2496,7 @@
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -2499,7 +2508,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -2516,7 +2525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>223</v>
       </c>
       <c r="C39" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D39" t="s">
         <v>82</v>
@@ -2567,7 +2576,7 @@
         <v>223</v>
       </c>
       <c r="C40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D40" t="s">
         <v>82</v>
@@ -2593,7 +2602,7 @@
         <v>223</v>
       </c>
       <c r="C41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D41" t="s">
         <v>82</v>
@@ -2619,7 +2628,7 @@
         <v>223</v>
       </c>
       <c r="C42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D42" t="s">
         <v>82</v>
@@ -2645,7 +2654,7 @@
         <v>223</v>
       </c>
       <c r="C43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43" t="s">
         <v>82</v>
@@ -2671,7 +2680,7 @@
         <v>223</v>
       </c>
       <c r="C44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" t="s">
         <v>82</v>
@@ -2697,7 +2706,7 @@
         <v>223</v>
       </c>
       <c r="C45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D45" t="s">
         <v>82</v>
@@ -2723,7 +2732,7 @@
         <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D46" t="s">
         <v>82</v>
@@ -2749,7 +2758,7 @@
         <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" t="s">
         <v>82</v>
@@ -2775,7 +2784,7 @@
         <v>224</v>
       </c>
       <c r="C48" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D48" t="s">
         <v>82</v>
@@ -2798,7 +2807,7 @@
         <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D49" t="s">
         <v>82</v>
@@ -2810,7 +2819,7 @@
         <v>11</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J49">
         <v>7.3999999999999996E-2</v>
@@ -2821,7 +2830,7 @@
         <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D50" t="s">
         <v>82</v>
@@ -2844,7 +2853,7 @@
         <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D51" t="s">
         <v>82</v>
@@ -2867,7 +2876,7 @@
         <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D52" t="s">
         <v>82</v>
@@ -2890,7 +2899,7 @@
         <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D53" t="s">
         <v>82</v>
@@ -2916,7 +2925,7 @@
         <v>251</v>
       </c>
       <c r="C54" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D54" t="s">
         <v>82</v>
@@ -2942,7 +2951,7 @@
         <v>251</v>
       </c>
       <c r="C55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D55" t="s">
         <v>82</v>
@@ -2965,7 +2974,7 @@
         <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D56" t="s">
         <v>82</v>
@@ -2988,10 +2997,10 @@
         <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D57" t="s">
         <v>82</v>
@@ -3003,10 +3012,10 @@
         <v>11</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="J57">
-        <v>5.7000000000000002E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3014,7 +3023,7 @@
         <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D58" t="s">
         <v>82</v>
@@ -3037,10 +3046,10 @@
         <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D59" t="s">
         <v>82</v>
@@ -3052,10 +3061,10 @@
         <v>11</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="J59">
-        <v>5.7000000000000002E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3063,7 +3072,7 @@
         <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D60" t="s">
         <v>82</v>
@@ -3086,7 +3095,7 @@
         <v>113</v>
       </c>
       <c r="C61" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D61" t="s">
         <v>82</v>
@@ -3109,7 +3118,7 @@
         <v>114</v>
       </c>
       <c r="C62" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D62" t="s">
         <v>82</v>
@@ -3121,7 +3130,7 @@
         <v>11</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J62">
         <v>3.1E-2</v>
@@ -3132,10 +3141,10 @@
         <v>126</v>
       </c>
       <c r="B63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D63" t="s">
         <v>82</v>
@@ -3147,7 +3156,7 @@
         <v>11</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J63">
         <v>0.11700000000000001</v>
@@ -3158,10 +3167,10 @@
         <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C64" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D64" t="s">
         <v>82</v>
@@ -3173,13 +3182,13 @@
         <v>11</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J64">
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -3213,7 +3222,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>175</v>
       </c>
@@ -3230,7 +3239,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -3247,7 +3256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>177</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>178</v>
       </c>
@@ -3281,7 +3290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -3298,7 +3307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>180</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>187</v>
       </c>
@@ -3329,7 +3338,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>191</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>192</v>
       </c>
@@ -3363,7 +3372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -3380,7 +3389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -3397,7 +3406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>195</v>
       </c>
@@ -3414,7 +3423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>196</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D80" t="s">
         <v>92</v>
@@ -3457,12 +3466,12 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D81" t="s">
         <v>92</v>
@@ -3488,7 +3497,7 @@
         <v>135</v>
       </c>
       <c r="C82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D82" t="s">
         <v>92</v>
@@ -3514,7 +3523,7 @@
         <v>136</v>
       </c>
       <c r="C83" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D83" t="s">
         <v>92</v>
@@ -3529,7 +3538,7 @@
         <v>208</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J83">
         <v>1.94</v>
@@ -3540,7 +3549,7 @@
         <v>94</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D84" t="s">
         <v>95</v>
@@ -3569,7 +3578,7 @@
         <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D85" t="s">
         <v>118</v>
@@ -3598,7 +3607,7 @@
         <v>98</v>
       </c>
       <c r="C86" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D86" t="s">
         <v>131</v>
@@ -3613,13 +3622,13 @@
         <v>134</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J86">
         <v>12.48</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -3641,7 +3650,7 @@
         <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D88" t="s">
         <v>86</v>
@@ -3664,7 +3673,7 @@
         <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D89" t="s">
         <v>86</v>
@@ -3687,7 +3696,7 @@
         <v>121</v>
       </c>
       <c r="C90" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D90" t="s">
         <v>86</v>
@@ -3705,7 +3714,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -3722,7 +3731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>144</v>
       </c>
@@ -3739,7 +3748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>145</v>
       </c>
@@ -3756,7 +3765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>146</v>
       </c>
@@ -3773,7 +3782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>147</v>
       </c>
@@ -3790,7 +3799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>148</v>
       </c>
@@ -3807,7 +3816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>149</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>150</v>
       </c>
@@ -3841,7 +3850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>167</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>169</v>
       </c>
@@ -3875,7 +3884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>170</v>
       </c>
@@ -3892,7 +3901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>171</v>
       </c>
@@ -3909,7 +3918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>172</v>
       </c>
@@ -3926,7 +3935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>199</v>
       </c>
@@ -3951,7 +3960,7 @@
         <v>151</v>
       </c>
       <c r="C105" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D105" t="s">
         <v>157</v>
@@ -3974,7 +3983,7 @@
         <v>152</v>
       </c>
       <c r="C106" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D106" t="s">
         <v>157</v>
@@ -3992,7 +4001,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>153</v>
       </c>
@@ -4009,7 +4018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>154</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>155</v>
       </c>
@@ -4043,7 +4052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>156</v>
       </c>
@@ -4068,7 +4077,7 @@
         <v>212</v>
       </c>
       <c r="C111" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D111" t="s">
         <v>163</v>
@@ -4086,7 +4095,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>161</v>
       </c>
@@ -4112,7 +4121,7 @@
         <v>0.72399999999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>203</v>
       </c>
@@ -4132,23 +4141,34 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I117" s="4" t="s">
         <v>214</v>
       </c>
       <c r="J117" s="5">
         <f>SUM(J2:J113)</f>
-        <v>77.393000000000015</v>
-      </c>
+        <v>77.90900000000002</v>
+      </c>
+      <c r="K117" s="5"/>
+      <c r="L117" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N113" xr:uid="{AE3DD381-F2B7-403A-B289-727EF6C0D84E}"/>
+  <autoFilter ref="A1:N113" xr:uid="{AE3DD381-F2B7-403A-B289-727EF6C0D84E}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="General"/>
+        <filter val="Input Attenuation Stage"/>
+        <filter val="JFET Buffer and Gain Stage"/>
+        <filter val="Output Stage"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I111" r:id="rId1" display="https://be.farnell.com/alps-alpine/sssf011700/slide-switch-spdt-0-1a-30v-tht/dp/3261774?st=switch%20slide" xr:uid="{D0D6BEF2-996F-4A06-B35A-02EEEC80A8AA}"/>
+    <hyperlink ref="I111" r:id="rId1" xr:uid="{D0D6BEF2-996F-4A06-B35A-02EEEC80A8AA}"/>
     <hyperlink ref="I112" r:id="rId2" display="https://be.farnell.com/alps-alpine/sssf011700/slide-switch-spdt-0-1a-30v-tht/dp/3261774?st=switch%20slide" xr:uid="{F442F32C-8502-42BE-AB56-A742441952D8}"/>
     <hyperlink ref="I113" r:id="rId3" display="https://be.farnell.com/pro-power/ppw01010/2-1mm-dc-socket-locking/dp/3498419?st=dc%20barrel%20jack" xr:uid="{8C7C4A37-7AA0-4906-AF82-90CF878D4023}"/>
-    <hyperlink ref="I85" r:id="rId4" display="https://be.farnell.com/renesas/hfa3046bz/transistor-npn-12v-0-15w-soic/dp/2983709?ost=hfa3046" xr:uid="{9EC2271E-74B8-4F63-945C-48C162315737}"/>
+    <hyperlink ref="I85" r:id="rId4" xr:uid="{9EC2271E-74B8-4F63-945C-48C162315737}"/>
     <hyperlink ref="I84" r:id="rId5" display="https://www.mouser.be/ProductDetail/InterFET/IFN411?qs=ggD623E1wpTqTvB4DJqgbw%3D%3D" xr:uid="{5465D79E-22EB-4CAB-AE87-A15EBCEDBA33}"/>
     <hyperlink ref="I39" r:id="rId6" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{3F3C68F7-2183-4729-9923-81D054D613B9}"/>
     <hyperlink ref="I40" r:id="rId7" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{52F3F128-6F80-4E7E-8496-5C05CA8B6E8E}"/>
@@ -4158,9 +4178,9 @@
     <hyperlink ref="I44" r:id="rId11" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{7F69FAAD-FFBF-4F81-82DD-3FD03116926E}"/>
     <hyperlink ref="I45" r:id="rId12" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{97983E24-B3F5-4F72-BEDD-0199498168E4}"/>
     <hyperlink ref="I46" r:id="rId13" display="https://be.farnell.com/neohm-te-connectivity/yr1b1m0cc/res-1m-0-10-250mw-axial-metal/dp/1083579?st=1m%20resistor" xr:uid="{6B2B45C4-DDA1-4F69-ADB1-D8463EED1C77}"/>
-    <hyperlink ref="I47" r:id="rId14" display="https://be.farnell.com/multicomp/mcmf0w4df2612a50/res-26k1-0-50-250mw-axial/dp/1563153" xr:uid="{641175BA-9D50-494D-A430-C85D7B350545}"/>
+    <hyperlink ref="I47" r:id="rId14" xr:uid="{641175BA-9D50-494D-A430-C85D7B350545}"/>
     <hyperlink ref="I48" r:id="rId15" display="https://be.farnell.com/multicomp/mcmf0w4df2612a50/res-26k1-0-50-250mw-axial/dp/1563153" xr:uid="{8B4EF911-20E9-4125-A430-3AE0C07DF73A}"/>
-    <hyperlink ref="I80" r:id="rId16" display="https://be.farnell.com/vishay/t93yb501kt20/trimmer-pot-500r-23turn-thd/dp/1141414?st=trimpot" xr:uid="{CD773C5A-2FF2-47B0-96ED-D7D84F9F24A8}"/>
+    <hyperlink ref="I80" r:id="rId16" xr:uid="{CD773C5A-2FF2-47B0-96ED-D7D84F9F24A8}"/>
     <hyperlink ref="I2" r:id="rId17" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{5760DDC1-F974-4B8F-8172-E6C89F2DC67A}"/>
     <hyperlink ref="I3" r:id="rId18" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{9B6162F1-074B-454D-AFDB-754BA66A8BA1}"/>
     <hyperlink ref="I4" r:id="rId19" display="https://www.mouser.be/ProductDetail/Vishay-Draloric/HSE682SAQCF0KR?qs=6lQ0QAtkVxmQt2Vp%252BwyNXA%3D%3D" xr:uid="{3EDED0DE-88D0-4B5E-8D01-6249EF594A0B}"/>
@@ -4175,44 +4195,45 @@
     <hyperlink ref="I14" r:id="rId28" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3AD820JYNNA?qs=2FIyTMJ0hNlY1vHleNE%252B0A%3D%3D" xr:uid="{A4E09FC9-1439-4787-A730-59EC72CE93A3}"/>
     <hyperlink ref="I11" r:id="rId29" display="https://www.mouser.be/ProductDetail/Knowles-Voltronics/JZ300?qs=l0I8jaqwYiDrMk2Sd%252BO3uQ%3D%3D" xr:uid="{6FDE52E5-E44A-47A3-BFA8-C79F8D07A0BE}"/>
     <hyperlink ref="I15" r:id="rId30" display="https://www.mouser.be/ProductDetail/Knowles-Voltronics/JZ300?qs=l0I8jaqwYiDrMk2Sd%252BO3uQ%3D%3D" xr:uid="{D05A97ED-9FA3-467A-B0E8-09B89E201259}"/>
-    <hyperlink ref="I88" r:id="rId31" display="https://be.farnell.com/on-semiconductor/1n4148tr/diode-100v-200ma-do-35/dp/9843680?st=1n4148" xr:uid="{29DDBB07-86F0-491F-B1DE-1595D1348EAA}"/>
+    <hyperlink ref="I88" r:id="rId31" xr:uid="{29DDBB07-86F0-491F-B1DE-1595D1348EAA}"/>
     <hyperlink ref="I89" r:id="rId32" display="https://be.farnell.com/on-semiconductor/1n4148tr/diode-100v-200ma-do-35/dp/9843680?st=1n4148" xr:uid="{DFE394BF-4AEC-4D75-97EF-94A70C1C8BE9}"/>
     <hyperlink ref="I17" r:id="rId33" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{B01CC1CC-D2FB-4484-99F2-69412A92765F}"/>
     <hyperlink ref="I20" r:id="rId34" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{41B0C811-66C8-4CD2-A5A2-A2DCD50CC5B0}"/>
     <hyperlink ref="I56" r:id="rId35" display="https://be.farnell.com/multicomp/mf25-680r/res-680r-1-250mw-axial-metal-film/dp/9342150?st=680r" xr:uid="{28487200-27F9-4A59-BAC5-90632C3EEFFC}"/>
-    <hyperlink ref="I58" r:id="rId36" display="https://be.farnell.com/multicomp/mf25-680r/res-680r-1-250mw-axial-metal-film/dp/9342150?st=680r" xr:uid="{91670B6C-416D-4DDA-9A00-1DA28BC684F6}"/>
+    <hyperlink ref="I58" r:id="rId36" xr:uid="{91670B6C-416D-4DDA-9A00-1DA28BC684F6}"/>
     <hyperlink ref="I21" r:id="rId37" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{244ADBF4-02F8-402E-8BB8-45639439037B}"/>
     <hyperlink ref="I22" r:id="rId38" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{E8A53E81-D234-491B-BB47-DD505F92D30A}"/>
     <hyperlink ref="I26" r:id="rId39" display="https://be.farnell.com/vishay/k104k15x7rf53h5/cap-0-1-f-50v-10-x7r/dp/1141777" xr:uid="{77B2FCC8-BE9C-4A9B-A869-D5D7FC6E803C}"/>
-    <hyperlink ref="I81" r:id="rId40" display="https://be.farnell.com/bi-technologies-tt-electronics/67wr1klf/trimmer-potentiometer-1kohm-20turn/dp/2113000" xr:uid="{87418403-41F6-45AB-BA12-04A436954BE9}"/>
-    <hyperlink ref="I50" r:id="rId41" display="https://be.farnell.com/vishay/mrs25000c3481fct00/res-3k48-1-600mw-axial-metal-film/dp/9467858?st=3k48" xr:uid="{17D09F55-78DB-4262-8545-3B06F0F1D349}"/>
-    <hyperlink ref="I51" r:id="rId42" display="https://be.farnell.com/vishay/mrs25000c4021fct00/res-4k02-1-600mw-axial-metal-film/dp/9468617" xr:uid="{B0AF7ABD-0420-46E7-9604-716253BB2062}"/>
-    <hyperlink ref="I54" r:id="rId43" display="https://be.farnell.com/tt-electronics-welwyn/mfr3-2k2fc/res-2k2-1-400mw-axial-metal-film/dp/1565301" xr:uid="{0350F701-4CA5-4971-983A-9AC313A8F313}"/>
+    <hyperlink ref="I81" r:id="rId40" xr:uid="{87418403-41F6-45AB-BA12-04A436954BE9}"/>
+    <hyperlink ref="I50" r:id="rId41" xr:uid="{17D09F55-78DB-4262-8545-3B06F0F1D349}"/>
+    <hyperlink ref="I51" r:id="rId42" xr:uid="{B0AF7ABD-0420-46E7-9604-716253BB2062}"/>
+    <hyperlink ref="I54" r:id="rId43" xr:uid="{0350F701-4CA5-4971-983A-9AC313A8F313}"/>
     <hyperlink ref="I55" r:id="rId44" display="https://be.farnell.com/tt-electronics-welwyn/mfr3-2k2fc/res-2k2-1-400mw-axial-metal-film/dp/1565301" xr:uid="{1F09C569-10A4-4B94-883E-C563074E8DA1}"/>
-    <hyperlink ref="I105" r:id="rId45" display="https://be.farnell.com/multicomp/2n2222a/transistor-npn-40v-800ma-to-18/dp/9207120?st=2n2222a" xr:uid="{9842300D-E100-4BD5-815A-CAFA573FC829}"/>
-    <hyperlink ref="I106" r:id="rId46" display="https://be.farnell.com/multicomp/2n2907a/transistor-pnp-60v-0-6a-to-18/dp/9206914?st=2n2907a" xr:uid="{F9A95863-5450-4C36-84C7-33DE6102C9B8}"/>
-    <hyperlink ref="I60" r:id="rId47" display="https://be.farnell.com/vishay/mrs25000c6200fct00/res-620r-1-600mw-axial-metal-film/dp/9469478" xr:uid="{CEF51342-B93E-47A6-BF8F-1804E8D958A0}"/>
-    <hyperlink ref="I90" r:id="rId48" display="https://be.farnell.com/multicomp/mcl034gd/led-3mm-70-green/dp/1581114?st=led%20green%203mm" xr:uid="{ED6F5F23-F913-4D65-A6CB-D5DEAE6ED496}"/>
+    <hyperlink ref="I105" r:id="rId45" xr:uid="{9842300D-E100-4BD5-815A-CAFA573FC829}"/>
+    <hyperlink ref="I106" r:id="rId46" xr:uid="{F9A95863-5450-4C36-84C7-33DE6102C9B8}"/>
+    <hyperlink ref="I60" r:id="rId47" xr:uid="{CEF51342-B93E-47A6-BF8F-1804E8D958A0}"/>
+    <hyperlink ref="I90" r:id="rId48" xr:uid="{ED6F5F23-F913-4D65-A6CB-D5DEAE6ED496}"/>
     <hyperlink ref="I61" r:id="rId49" display="https://be.farnell.com/tt-electronics-welwyn/mfr3-6k8fc/res-6k8-1-400mw-axial-metal-film/dp/1565329" xr:uid="{E025BA6F-62AA-4F86-B6B7-BAF8F06CA034}"/>
     <hyperlink ref="I18" r:id="rId50" display="https://www.mouser.be/ProductDetail/Vishay-BC-Components/D680J25SL0L6UJ5R?qs=zbK%252Bn7%2FlzNe0KfHTjMNtBQ%3D%3D" xr:uid="{8AC611E2-D3A4-4F80-A3CE-534B8C748163}"/>
-    <hyperlink ref="I82" r:id="rId51" display="https://be.farnell.com/bourns/3362p-1-501lf/trimmer-500r/dp/9354360" xr:uid="{BED028FA-29B4-4D4F-B954-517B2B3F4962}"/>
-    <hyperlink ref="I52" r:id="rId52" display="https://be.farnell.com/vishay/mrs25000c3740fct00/res-374r-1-600mw-axial-metal-film/dp/9467602?st=374r" xr:uid="{D731766B-C266-4865-B49A-39E4D2135AC3}"/>
-    <hyperlink ref="I53" r:id="rId53" display="https://be.farnell.com/multicomp/mcre000052/res-18k-5-125mw-axial-carbon-film/dp/1700254" xr:uid="{36917585-E2FC-4503-A438-6626DCC4BA53}"/>
+    <hyperlink ref="I82" r:id="rId51" xr:uid="{BED028FA-29B4-4D4F-B954-517B2B3F4962}"/>
+    <hyperlink ref="I52" r:id="rId52" xr:uid="{D731766B-C266-4865-B49A-39E4D2135AC3}"/>
+    <hyperlink ref="I53" r:id="rId53" xr:uid="{36917585-E2FC-4503-A438-6626DCC4BA53}"/>
     <hyperlink ref="I19" r:id="rId54" display="https://www.mouser.be/ProductDetail/TDK/CC45SL3DD330JYGNA?qs=eSfX1CQlHqpvQOwssXPbQg%3D%3D" xr:uid="{834E95C5-E47C-45AC-B177-2591B992DDFB}"/>
-    <hyperlink ref="I57" r:id="rId55" display="https://be.farnell.com/te-connectivity/lr1f2r21/res-2r21-1-600mw-axial-metal-film/dp/2330096?st=210r" xr:uid="{B2742A17-62A9-4FAC-A418-547B8704876F}"/>
-    <hyperlink ref="I59" r:id="rId56" display="https://be.farnell.com/te-connectivity/lr1f2r21/res-2r21-1-600mw-axial-metal-film/dp/2330096?st=210r" xr:uid="{C119CABC-C870-49E1-B8BA-9A3EF2CE2F21}"/>
-    <hyperlink ref="I62" r:id="rId57" display="https://be.farnell.com/multicomp/mf12-510r/res-510r-1-125mw-axial-metal-film/dp/9343300?st=510r" xr:uid="{3477097F-1ED6-4EC1-8948-3A591088C375}"/>
-    <hyperlink ref="I23" r:id="rId58" display="https://www.mouser.be/ProductDetail/Vishay-BC-Components/D103K43Y5PH6TJ5R?qs=wEmTtUuRSe6NCZwQxzdYuQ%3D%3D" xr:uid="{F8DF7D0C-8FE8-4C1E-8475-0B667D46C7EF}"/>
-    <hyperlink ref="I64" r:id="rId59" display="https://be.farnell.com/vishay/mrs25000c4421fct00/res-4k42-1-600mw-axial-metal-film/dp/9468668?st=4k42" xr:uid="{F78F9488-DD3E-4D6D-B81A-7D9463AFF13C}"/>
-    <hyperlink ref="I63" r:id="rId60" display="https://be.farnell.com/vishay/mrs25000c4421fct00/res-4k42-1-600mw-axial-metal-film/dp/9468668?st=4k42" xr:uid="{F3319D17-125B-46B6-B7B5-7BC4DD70F34D}"/>
-    <hyperlink ref="I25" r:id="rId61" display="https://www.mouser.be/ProductDetail/Vishay-Cera-Mite/561R10TCCV68BA?qs=XeJOwCSCkv%252BIxAC3i6sxEw%3D%3D" xr:uid="{077D24FE-23E1-41F0-817A-318050C65A80}"/>
-    <hyperlink ref="I86" r:id="rId62" display="https://be.farnell.com/analog-devices/ad797anz/ic-op-amp-u-low-noise-dip8-797/dp/9603778?st=ad797" xr:uid="{51E3E616-BCC4-4F12-87FF-E95E5C233D6F}"/>
-    <hyperlink ref="I83" r:id="rId63" display="https://be.farnell.com/vishay/m64w104kb40/trimmer-pot-100k-23turn-thd/dp/9608656" xr:uid="{93E55DA0-91AF-4E4A-A212-91DF39EA83FE}"/>
-    <hyperlink ref="I49" r:id="rId64" display="https://be.farnell.com/te-connectivity/lr1f7r5/res-7r5-1-600mw-axial-metal-film/dp/2330224?st=7r5" xr:uid="{4164D69A-50B6-4B68-AD5E-3A0B5E55902B}"/>
-    <hyperlink ref="I16" r:id="rId65" display="https://www.mouser.be/ProductDetail/Vishay/1C10C0G220J050B?qs=%2FVYrxewl4mYopKLzL8PbyA%3D%3D" xr:uid="{1644BCB7-E1ED-4CA8-A1DB-0C4A423E4ABF}"/>
+    <hyperlink ref="I62" r:id="rId55" xr:uid="{3477097F-1ED6-4EC1-8948-3A591088C375}"/>
+    <hyperlink ref="I23" r:id="rId56" display="https://www.mouser.be/ProductDetail/Vishay-BC-Components/D103K43Y5PH6TJ5R?qs=wEmTtUuRSe6NCZwQxzdYuQ%3D%3D" xr:uid="{F8DF7D0C-8FE8-4C1E-8475-0B667D46C7EF}"/>
+    <hyperlink ref="I64" r:id="rId57" display="https://be.farnell.com/vishay/mrs25000c4421fct00/res-4k42-1-600mw-axial-metal-film/dp/9468668?st=4k42" xr:uid="{F78F9488-DD3E-4D6D-B81A-7D9463AFF13C}"/>
+    <hyperlink ref="I63" r:id="rId58" xr:uid="{F3319D17-125B-46B6-B7B5-7BC4DD70F34D}"/>
+    <hyperlink ref="I25" r:id="rId59" display="https://www.mouser.be/ProductDetail/Vishay-Cera-Mite/561R10TCCV68BA?qs=XeJOwCSCkv%252BIxAC3i6sxEw%3D%3D" xr:uid="{077D24FE-23E1-41F0-817A-318050C65A80}"/>
+    <hyperlink ref="I86" r:id="rId60" display="https://be.farnell.com/analog-devices/ad797anz/ic-op-amp-u-low-noise-dip8-797/dp/9603778?st=ad797" xr:uid="{51E3E616-BCC4-4F12-87FF-E95E5C233D6F}"/>
+    <hyperlink ref="I83" r:id="rId61" xr:uid="{93E55DA0-91AF-4E4A-A212-91DF39EA83FE}"/>
+    <hyperlink ref="I49" r:id="rId62" xr:uid="{4164D69A-50B6-4B68-AD5E-3A0B5E55902B}"/>
+    <hyperlink ref="I16" r:id="rId63" display="https://www.mouser.be/ProductDetail/Vishay/1C10C0G220J050B?qs=%2FVYrxewl4mYopKLzL8PbyA%3D%3D" xr:uid="{1644BCB7-E1ED-4CA8-A1DB-0C4A423E4ABF}"/>
+    <hyperlink ref="I24" r:id="rId64" display="https://www.mouser.be/ProductDetail/Vishay-Cera-Mite/561R10TCCV68BA?qs=XeJOwCSCkv%252BIxAC3i6sxEw%3D%3D" xr:uid="{B058BED5-4ECD-44DC-831D-2395042A0A51}"/>
+    <hyperlink ref="I57" r:id="rId65" display="https://www.mouser.be/ProductDetail/Yageo/MFR-25FBF52-210R?qs=oAGoVhmvjhwWKFUNNlqasw%3D%3D" xr:uid="{3E05D82D-9B4F-4249-8477-A5B6EA15B04E}"/>
+    <hyperlink ref="I59" r:id="rId66" display="https://www.mouser.be/ProductDetail/Yageo/MFR-25FBF52-210R?qs=oAGoVhmvjhwWKFUNNlqasw%3D%3D" xr:uid="{1E8DA22A-83B3-444F-A086-990A81D9D4C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
+  <pageSetup paperSize="9" scale="44" fitToHeight="0" orientation="landscape" r:id="rId67"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>